<commit_message>
Updated with 2025-F data from FT
</commit_message>
<xml_diff>
--- a/output/results_llm_lda_topics.xlsx
+++ b/output/results_llm_lda_topics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B126"/>
+  <dimension ref="A1:B130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1945,6 +1945,54 @@
         </is>
       </c>
     </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-F_Topic 0</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Politisk debat om indfødsret og statsborgerskab i Danmark</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-F_Topic 1</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Debat om statsborgerskab og integrationspolitik i Danmark</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-F_Topic 2</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Debatten om statsborgerskab og indvandringspolitik i Danmark</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-F_Topic 3</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Politisk Debat om Udlændingepolitik og Identitet i Danmark</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Redid LDA topics based on new prompt
</commit_message>
<xml_diff>
--- a/output/results_llm_lda_topics.xlsx
+++ b/output/results_llm_lda_topics.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Den danske indvandringspolitik og indfødsretslovgivning er genstand for intens debat, hvor der efterlyses strammere sprogkrav og en kritisk revurdering af integrationsmetoderne, mens der samtidig ses uenighed mellem partierne om kravene til statsborgerskab og håndteringen af ansøgere. Diskussionen fremhæver skillelinjer mellem politiske partier, især vedrørende Dansk Folkepartis retorik og Socialdemokratiets syn på statsborgerskab, samt behovet for mere gennemsigtighed og rimelighed i beslutningsprocessen.</t>
+          <t>Debatten om Danmarks indvandrings- og integrationspolitik fokuserer på kravene til sprogkundskaber og indfødsret, der skaber politisk splittelse og behov for strammere regler for at beskytte dansk identitet.</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Diskussionen om diskrimination og lighed er præget af uenighed om indvandringspolitikken, hvor venstrefløjen kritiseres for sin tilgang til lighed mellem danske borgere og fremmede, mens Kristendemokraterne efterlyser en ny aftale om indfødsret, der respekterer tidligere principper og anerkender forskellen mellem indfødsret og permanent opholdstilladelse.</t>
+          <t>Diskussionen om diskrimination og lighed centrerer sig om indvandringspolitikken og uenigheder om, hvordan man skal forholde sig til indfødsret og permanent opholdstilladelse i forhold til danske borgere og fremmede.</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Stramningen af betingelserne for dansk indfødsret sigter mod at sikre, at kun værdige ansøgere opnår statsborgerskab, men der er behov for større gennemsigtighed i lovgivningsprocessen og en mere retfærdig behandling af ansøgere, da nuværende procedurer skaber udfordringer i samfundet. Det Radikale Venstre støtter, at kvalificerede ansøgere skal have statsborgerskab, men kritiserer Dansk Folkepartis begrænsninger, der komplicerer processen.</t>
+          <t>Der er behov for strammere betingelser og mere gennemsigtighed i dansk indfødsret for at sikre samfundets sammenhængskraft og håndtere udfordringer relateret til indvandrere, samtidig med at ansøgere, der opfylder kravene, bør have ret til dansk statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Høje boglige krav kan udgøre en hindring for indvandrere, der ønsker at blive selvforsørgende, og der er behov for at beskytte borgerlige frihedsrettigheder som lighed for loven og forbud mod diskrimination fra religiøs debat.</t>
+          <t>Høje boglige krav kan være en hindring for indvandrere, der ønsker selvforsørgelse, og lighed for loven samt forbud mod diskrimination er centrale borgerlige frihedsrettigheder.</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lovforslaget om tildeling af dansk statsborgerskab til personer med langvarig ophold og sprogkvalifikationer understreger vigtigheden af integration i det danske samfund, samtidig med at der diskuteres forskellige holdninger til indfødsretsbehandling og forholdet mellem historisk viden og terrorisme.</t>
+          <t>Der er en anbefaling om at godkende lovforslaget om dansk statsborgerskab for langvarige beboere, med fokus på integration og sprogkrav, samtidig med kritik af Dansk Folkepartis syn på indfødsret og integration.</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Der stilles spørgsmål ved det danske tankesæt og Dansk Folkepartis holdning til sprogkravet for indfødsret.</t>
+          <t>Der stilles spørgsmål ved det danske tankesæt og Dansk Folkepartis holdning til dispensation fra sprogkravet for indfødsret.</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Indfødsret er vigtig for at opretholde dansk identitet og kultur, og kravene til dansk statsborgerskab bør skærpes for at sikre nye borgeres bidrag til fællesskabet uden at gå på kompromis med danske værdier og sikkerhed. Tildeling af indfødsret bør ikke betragtes som en løsning for personer med psykiske lidelser.</t>
+          <t>Indfødsret er afgørende for at bevare dansk identitet og kultur, og kravene til statsborgerskab bør skærpes for at sikre nye borgeres bidrag til fællesskabet.</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Der er alvorlige retssikkerhedsmæssige problemer i tildelingen af dansk statsborgerskab, da praksis strammes og ansøgninger ofte afvises uden begrundelse, hvilket kan føre til eksklusion af ansøgere, mens Det Radikale Venstre opfordrer til en mere retfærdig behandling og fokus på at hjælpe sårbare grupper. Lovforslaget berører en stor gruppe mennesker fra forskellige lande, hvilket understreger kompleksiteten i ansøgningsprocessen.</t>
+          <t>Der er alvorlige problemer med retssikkerheden i tildelingen af dansk statsborgerskab, præget af afvisninger uden begrundelse og stramninger, som kan føre til eksklusion og radikalisering af ansøgere, mens der er behov for mere ensartet behandling og fokus på at hjælpe udsatte grupper.</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Danmark oplever en folkevandringstid med mange ansøgere til statsborgerskab, hvor der forventes tilpasning og respekt for danske værdier, understøttet af krav til sprog og kulturforståelse.</t>
+          <t>Danmark oplever en folkevandring med mange ansøgere til statsborgerskab, hvor der forventes tilpasning til danske værdier og krav om sprogkundskaber.</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lovforslaget om indfødsret i Danmark illustrerer den komplekse og uretfærdige natur af lovgivningen, især for torturofre, samtidig med at der fremsættes et ændringsforslag for en fejlagtigt registreret pige. Det Konservative Folkeparti kritiseres for manglende handling vedrørende asylbørns vilkår og indfødsretsaftalen, hvilket rejser spørgsmål om menneskelighed i Udlændingeservice.</t>
+          <t>Lovforslaget om indfødsret i Danmark belyser kompleksiteten og uretfærdigheden i lovgivningen, især for sårbare grupper som torturofre og asylbørn, samtidig med at der fremsættes ændringsforslag for at rette fejl i registreringen af statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Der er en bestræbelse på at finde løsninger for at give børn dansk statsborgerskab, især i tilfælde af fejlregistreringer eller manglende opmærksomhed.</t>
+          <t>Der er en vilje til at finde løsninger for at give børn dansk statsborgerskab, især i tilfælde af fejlregistreringer eller manglende opmærksomhed.</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Der er uenighed mellem taleren og hr. Jørgen Arbo-Bæhr om indfødsrettens betingelser, hvor taleren afviser, at sygdom kan retfærdiggøre statsborgerskab og påpeger vigtigheden af at anerkende en nation og folk samt kravene om dansk sprog og lovgivernes vurdering.</t>
+          <t>Der er uenighed om indfødsret, hvor taleren mener, at sygdom ikke kan legitimere statsborgerskab, og at anerkendelse af folk og nation er vigtig.</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Det Radikale Venstre fejrer nye danske statsborgere, men kritiserer indfødsretsaftalen og kravene, især for torturofre og danskhedstest, og mener, at der bør være mulighed for dispensation samt evaluering af kravene for bedre integration.</t>
+          <t>Det Radikale Venstre støtter nye danske statsborgere, men ønsker ændringer i indfødsretsaftalen og kravene til statsborgerskab for at fremme integrationen.</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Der opfordres til at byde nye statsborgere velkommen og anerkende deres engagement i det danske demokrati, samtidig med at kritik rettes mod lovforslaget, der udelukker visse grupper, herunder personer med PTSD, fra dispensation fra kravene for statsborgerskab, hvilket anses for en uretfærdig begrænsning af deres rettigheder.</t>
+          <t>Der opfordres til at byde nye statsborgere velkommen og anerkende deres engagement i det danske samfund, samtidig med at der kritiseres for uretfærdige begrænsninger i statsborgerskabsprocessen, særligt for dem med psykiske lidelser.</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Den konservative folketingsgruppe understreger vigtigheden af rimelige krav for dansk statsborgerskab, samtidig med at de anerkender behovet for dispensationer, men kritiserer den nye indfødsretsaftale for ikke at tage højde for væsentlige problemstillinger som torturofre.</t>
+          <t>Den konservative folketingsgruppe støtter rimelige krav og særlige dispensationer for dansk statsborgerskab, men kritiserer den nye indfødsretsaftale for ikke at adressere vigtige problemstillinger.</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Samarbejdet mellem Det Konservative Folkeparti og Venstre i Indfødsretsudvalget er positivt, men der er behov for klare krav til dansk sprogkundskab for statsborgerskab, hvor dispensation for posttraumatisk stress-syndrom ikke længere er automatisk og kræver en grundigere vurdering. Der efterlyses en holdning fra Helge Adam Møller om, hvorvidt psykiske lidelser bør behandles med samme hensyn som fysiske skader i relation til dansk sprogkrav.</t>
+          <t>Der er behov for klare krav til dansk sprogkundskab for statsborgerskab, og muligheden for dispensation ved posttraumatisk stress-syndrom skal vurderes grundigere.</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Lovforslaget vil give dansk statsborgerskab til cirka 1.800 personer, men Socialdemokraterne ønsker at rette op på, at 120 personer er blevet forhindret i at blive indstillet på grund af forsinkelse af indfødsretsprøven.</t>
+          <t>Lovforslaget vil give cirka 1.800 personer, herunder over 1.000 børn, dansk statsborgerskab, men der er problemer med indfødsretsprøven, som Socialdemokraterne ønsker at løse.</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Der er bekymring for, at omgåelse af indfødsretsprøven for 120 personer vil være uretfærdig over for fremtidige ansøgere, og der efterlyses en mere seriøs tilgang til håndteringen af prøven i stedet for hurtige løsninger.</t>
+          <t>Der er bekymring for en uretfærdig håndtering af indfødsretsprøven, og der efterlyses seriøst arbejde i stedet for hurtige løsninger.</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Statsborgerskabsdagen fejrede nye danske statsborgere, men der er frustration over strenge regler, der forhindrer 120 personer i at opnå statsborgerskab, hvilket rejser bekymringer om fremtidige begrænsninger og integration. Enhedslisten kritiserer de uforståelige bestemmelser, der hæmmer rettigheder og muligheder for nye statsborgere.</t>
+          <t>Statsborgerskabsdagen fejrer nye danskere, men der er bekymring og frustration over strenge regler, der begrænser tildelingen af dansk statsborgerskab og integration.</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Lovforslaget om indfødsret godkendes med ændringer, der fokuserer på dansk kultur og historie, mens dobbelt statsborgerskab afvises for at beskytte dansk identitet.</t>
+          <t>Lovforslaget om indfødsret godkendes med fokus på dansk kultur og historie, men der er bekymringer om tidligere indhold og afvisning af dobbelt statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Fru Hanne Agersnaps repræsentant lykønsker kommende danske statsborgere og understreger vigtigheden af integration, mens der kritiseres de skærpede krav for statsborgerskab, som kan gøre det vanskeligere for bidragsydere til samfundet at opnå det.</t>
+          <t>Repræsentanten lykønsker kommende statsborgere og fremhæver vigtigheden af integration, mens der kritiseres de skærpede krav for statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>I dag får 2.315 voksne og 810 børn dansk statsborgerskab, hvilket understreger vigtigheden af integration og respekt for deres valg om at skifte identitet.</t>
+          <t>En betydningsfuld dag for 2.315 voksne og 810 børn, der opnår dansk statsborgerskab, hvilket understreger vigtigheden af integration og respekt for deres identitetsvalg.</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Søren Krarup kritiserer den langsomme implementering af indfødsretsaftalen og fastholder kravene til sprogprøven, mens Morten Østergaard argumenterer for dispensation til personer med posttraumatisk stress for at fremme integration og kritiserer ændringer i vurderingsprocessen, der ignorerer lægelige hensyn.</t>
+          <t>Der er delte meninger om kravene til sprogprøven og vurderingsprocessen for indfødsret, hvor nogle mener, at kravene er rimelige, mens andre kalder på mere fleksibilitet for at fremme integration.</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Morten Østergaard fremhæver sin forventning om meddelelse om indfødsret baseret på tidligere kommunikation fra ministeren, mens Anne-Marie Meldgaard støtter lovforslaget om dansk statsborgerskab og anerkender dets betydning for ansøgerne samt de forpligtelser, der følger med statsborgerskabet.</t>
+          <t>Både Morten Østergaard og Anne-Marie Meldgaard understreger vigtigheden af indfødsret og de konsekvenser, det har for ansøgerne.</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Bekymringer over indfødsret til personer med arabiske navne afspejler både frygt for kulturel afstand og håb om positivt bidrag til samfundet, mens politiske partier som Det Radikale Venstre og Socialdemokratiet har forskellige syn på integrationskrav og anerkender de nye statsborgeres indsats.</t>
+          <t>Der er bekymringer og håb omkring indfødsret for personer med arabiske navne, samt en debat om kravene til statsborgerskab og integration i det danske samfund.</t>
         </is>
       </c>
     </row>
@@ -753,7 +753,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ministerens erkendelse af, at mange danskere har svært ved at opfylde kravene for statsborgerskab, står i kontrast til regeringens beslutning om at skærpe integrationsreglerne, til trods for anbefalinger om at lempe dem for at fremme integrationen.</t>
+          <t>Ministerens erkendelse af vanskelighederne ved at opnå dansk statsborgerskab står i kontrast til regeringens beslutning om at skærpe integrationsreglerne.</t>
         </is>
       </c>
     </row>
@@ -765,7 +765,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>En elev fra en handelsskole bliver lettet over at erfare, at dansk statsborgerskab kræver sprogkundskaber, viden om Danmark og en ordentlig livsførelse, hvilket fører til refleksion over indfødsret og støtte til indfødsretsprøven for at sikre værdige statsborgerskabsansøgere.</t>
+          <t>Diskussionen om dansk statsborgerskab fokuserer på kravene til sprogkundskaber, viden om Danmark og ordentlig livsførelse, samt betydningen af indfødsret og konsekvenserne af dobbelt statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Lovforslaget L 191 omhandler tildeling af dansk statsborgerskab til borgere, der ønsker at integrere sig i det danske samfund, samtidig med at der er en misforståelse omkring dobbelt statsborgerskab, som lovgivningen forbyder. Derudover udtrykker Venstre håb om, at de nye statsborgere vil deltage i statsborgerskabsdagen for at fejre deres nye status.</t>
+          <t>Lovforslaget L 191 omhandler tildeling af dansk statsborgerskab til borgere, der ønsker at blive en del af det danske samfund, samtidig med at der er misforståelser omkring dobbelt statsborgerskab og dets konsekvenser for dansk identitet.</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Den 26. april fejrede ca. 1.500 nytilkomne danske statsborgere deres opnåelse af statsborgerskab, hvilket markerer en vigtig sejr for demokratiet og sikrer dem fuldgyldige rettigheder, herunder stemmeret.</t>
+          <t>Den 26. april fejrede 1.500 nytilkomne danske statsborgere deres opnåede statsborgerskab, hvilket understreger vigtigheden af demokratisk deltagelse og rettigheder.</t>
         </is>
       </c>
     </row>
@@ -801,7 +801,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Dansk statsborgerskab giver tryghed til usikre personer, men der er misforståelser omkring kravene til opgivelse af tidligere statsborgerskaber, hvilket fremhæves i relation til flygtningestatus. Derudover anerkendes initiativet om en statsborgerskabsdag, mens det pointeres, at danske embedsmænd strengt følger lovgivningen i ansøgningsprocessen.</t>
+          <t>Dansk statsborgerskab giver tryghed til usikre personer, men der er misforståelser om kravene, herunder opgivelse af tidligere statsborgerskaber, og danske embedsmænd følger lovgivningen uden at tage hensyn til følelser i ansøgningsprocessen.</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Ministerens påstand om Troels G. Jørgensens rolle i kommunistlovgivningen er misvisende, da det var den tyske besættelsesmagt, der pålagde dette, og der argumenteres for, at Folketinget bør have mere selvbestemmelse over indfødsret uden internationale indblandinger.</t>
+          <t>Der apporteres om behovet for Folketingets selvbestemmelse over indfødsret og afvisning af ministerens påstand om kommunistlovgivningens oprindelse.</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Debatten om indfødsret i Danmark centrerer sig om konflikten mellem danske lovkrav og internationale FN-konventioner, hvor kritikere hævder, at indførelsen af statsborgerskab til personer, der ikke opfylder nationale krav, underminerer grundloven og Folketingets suverænitet, mens regeringen fremhæver betydningen af internationalt samarbejde. Der opstilles spørgsmål om, hvilke retsprincipper der skal prioriteres, og der argumenteres for, at beslutninger vedrørende opsigelse af konventioner bør ske med Folketingets flertal.</t>
+          <t>Debatten om indfødsret i Danmark fokuserer på konflikten mellem opfyldelse af internationale konventioner og beskyttelse af grundloven samt Folketingets suverænitet i beslutninger om statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Flere partier i Folketinget støtter et lovforslag om tildeling af dansk statsborgerskab til 1.736 personer, men kritiserer samtidig eksisterende praksisser, herunder kravet om at opgive oprindeligt statsborgerskab og FN's indflydelse på indfødsret. Dansk Folkeparti advarer om, at fremtidige tildelinger kan blive afvist, hvis kravene ikke respekteres.</t>
+          <t>Der er en fælles støtte til lovforslaget om dansk indfødsret, men samtidig en kritik af kravene og praksis omkring statsborgerskab, herunder ønsket om at tillade dobbelt statsborgerskab og bevare Folketingets autoritet i beslutningsprocessen.</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Ayaan Hirsi Ali diskuterer betydningen af loyalitet og respekt for danske værdier i forbindelse med tildeling af statsborgerskab, mens Danmark byder velkommen til nye statsborgere under et lovforslag, der også adresserer udfordringerne ved krav om at opgive oprindeligt statsborgerskab. Indfødsretsprøven understreger nødvendigheden af at have et solidt kendskab til Danmark for at sikre en vellykket integration.</t>
+          <t>Teksten omhandler tildeling af dansk statsborgerskab, vigtigheden af troskab over for danske værdier, og de krav og forberedelser, der er nødvendige for at blive statsborger i Danmark.</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Venstre og Liberal Alliance kritiserer justitsministerens håndtering af lovforslaget om statsborgerskab, især med fokus på retssikkerhed, demokratisk praksis og den potentielle belønning af personer med alvorlig kriminalitet. Der rejses bekymringer om ministerens manglende vilje til at støtte ændringsforslag og sikre en åben debat, hvilket skaber spørgsmål om integriteten af PET's vurderinger.</t>
+          <t>Der er bekymringer om demokratisk praksis og retssikkerhed i forbindelse med lovforslaget om statsborgerskab, herunder eksklusion af personer, PET's integritet og ministerens manglende svar på vigtige spørgsmål.</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Debatten i Folketinget om indfødsretslovforslaget afslører et dilemma mellem Danmarks sikkerhed og overholdelse af internationale konventioner, hvor Dansk Folkeparti prioriterer national sikkerhed og grundlovens principper, mens andre partier som Enhedslisten og Socialdemokratiet ønsker at lette adgangen til statsborgerskab for statsløse og dem, der opfylder kravene. Der er en bred enighed blandt flere partier om behovet for at revidere nuværende regler og sikre, at nationale sikkerhedsinteresser bliver prioriteret, samtidig med at der skal tages hensyn til internationale forpligtelser.</t>
+          <t>Debatten i Folketinget omhandler balancen mellem Danmarks sikkerhed og overholdelsen af internationale konventioner, hvor der er delte meninger om håndtering af statsborgerskab for personer, der anses for sikkerhedstrusler.</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tom Behnke kritiserer Venstre for at udvise manglende tillid til efterretningstjenesten og opfordrer regeringen til at ændre internationale konventioner for bedre at kunne håndtere sikkerhedstrusler, samtidig med at han roser De Konservative for deres principfaste holdning. Der er en bekymring for, at personer med alvorlig kriminalitet, som vurderes som sikkerhedsrisiko, kan opnå dansk statsborgerskab, hvilket kræver offentlig oplysning.</t>
+          <t>Der er enighed om den nuværende retstilstand vedrørende efterretningstjenesten, men bekymringer om håndtering af sikkerhedsrisici og behovet for ændringer i konventioner diskuteres.</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Venstre kritiserer regeringen for at ignorere anbefalinger fra Politiets Efterretningstjeneste om statsborgerskab og understreger behovet for reformer, der gør kravene til statsborgerskab mere tilgængelige, samtidig med at de fastholder, at personer med alvorlig kriminalitet ikke bør tildeles statsborgerskab. Der er en opfordring til, at Folketinget og justitsministeren anerkender problemerne ved nuværende retningslinjer og arbejder hen imod ændringer, især i relation til Danmarks internationale forpligtelser.</t>
+          <t>Der er enighed om nødvendigheden af at reformere statsborgerskabs krav, sikre integration af nye danskere og følge Politiets Efterretningstjenestes anbefalinger for at beskytte rigets sikkerhed, samtidig med at der er bekymringer om håndteringen af statsborgerskab for kriminelle.</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SF byder velkommen til nye statsborgere i Danmark, mens der stilles spørgsmål ved sagsbehandlingen og overholdelsen af regler, og Socialdemokratiet anerkender indsatsen for at opnå statsborgerskab gennem et nyt lovforslag. Diskussionen inkluderer også kritik af tidligere samarbejde med regeringen og tak til integrationsministeren.</t>
+          <t>SF og Socialdemokratiet byder nye statsborgere velkommen, men rejser spørgsmål om sagsbehandling og ønsket om klarhed over procedurerne.</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Dansk Folkeparti afviser loven om indfødsrets meddelelse, idet de mener, at den krænker grundlovens § 44 og underminerer Folketingets myndighed, hvilket de anser som et grundlovsbrud og et forræderi mod dansk selvstændighed.</t>
+          <t>Dansk Folkeparti afviser loven om indfødsrets meddelelse, da de mener, den krænker grundloven og underminerer Folketingets myndighed.</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Konservative støtter lovforslaget om dansk statsborgerskab for personer, der har opfyldt kravene, og understreger vigtigheden af at anerkende ansøgere, der stræber efter at blive danske statsborgere, samtidig med at de opfordrer til bred politisk opbakning.</t>
+          <t>Konservative støtter lovforslaget om dansk statsborgerskab for dem, der opfylder kravene, og fremhæver vigtigheden af at anerkende ansøgeres bestræbelser og sikre politisk opbakning.</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Lovforslaget om automatisk statsborgerskab til statsløse personer uden krav har mødt kritik for at være uretfærdigt over for dem, der har arbejdet for deres statsborgerskab, samt for at kunne belønne potentielle kriminelle, samtidig med at der udtrykkes glæde over at byde nye statsborgere velkommen og en anerkendelse af behovet for at bekæmpe statsløshed i Danmark. Der er også en debat om, hvordan personer født og opvokset i Danmark bør behandles anderledes i forhold til statsborgerskab.</t>
+          <t>Lovforslaget om automatisk tildeling af statsborgerskab til statsløse personer er både kritiseret og bifaldet, hvilket rejser spørgsmål om retfærdighed, sikkerhed og behandling af personer født i Danmark.</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Danmark tildeler statsborgerskab til 1.157 voksne og 487 børn, hvilket anerkender deres tilknytning til landet og giver dem en dansk identitet, mens politiske partier som Venstre og Liberal Alliance understreger vigtigheden af at behandle ansøgninger hurtigt for at undgå usikkerhed for ansøgerne. Lovforslagene sigter mod at bidrage til at udrydde statsløshed blandt personer, der allerede er en del af det danske samfund.</t>
+          <t>Statsborgerskab tildeles 1.157 voksne og 487 børn i Danmark, hvilket anerkender deres tilknytning til landet og sikrer deres danske identitet.</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Der er en stigende interesse blandt udlændinge for at opnå dansk statsborgerskab, men bekymringer omkring statsløse personer og deres sikkerhed skaber politiske spændinger, især med Dansk Folkepartis modstand mod at give statsborgerskab uden at opfylde de samme krav som andre. Diskussionen fokuserer på balancen mellem at inkludere statsløse i statsborgerskabsprogrammet og at sikre danskernes tryghed og krav om lighed i betingelserne for statsborgerskab.</t>
+          <t>Der er en debat om tildeling af dansk statsborgerskab til udlændinge, især statsløse, hvor bekymringer om sikkerhed og krav til ansøgere står centralt, samtidig med at der er anerkendelse af betydningen af aktiv deltagelse i civilsamfundet.</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Teksten fokuserer på betydningen af dansk statsborgerskab og den stolthed, nye statsborgere oplever, mens der samtidig diskuteres politiske holdninger til statsborgerskab, herunder Dansk Folkepartis krav og Enhedslistens støtte til lovforslaget om mere rimelige indfødsretsregler.</t>
+          <t>Der er en fælles stræben efter at forbedre adgangen til dansk statsborgerskab og udrydde statsløshed, samtidig med at forskellige politiske partier har forskellige holdninger til indfødsret og krav til medlemskab.</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Regeringen og et flertal i Folketinget kritiseres for at tildele statsborgerskab til kriminelle statsløse uden de samme krav som for andre ansøgere, hvilket både Dansk Folkeparti og Venstre finder moralsk forkasteligt og problematisk, især i forhold til sikkerhedsrisici. Begge partier opfordrer til ændringer for at undgå fremtidige konflikter omkring statsborgerskabsansøgninger.</t>
+          <t>Regeringen og Folketinget kritiseres for at tildele statsborgerskab til kriminelle statsløse uden samme krav som andre ansøgere, hvilket skaber bekymringer om sikkerhed og moral.</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Folketingets tildeling af dansk statsborgerskab til personer vurderet som sikkerhedsrisiko af Politiets Efterretningstjeneste rejser bekymringer om fortolkningen af internationale konventioner og har medført ændringer i Venstres holdning til integration, samtidig med at der er skuffelse over regeringens modvilje til at diskutere en ny fortolkning af FN-konventionen om statsløshed. Der opfordres til mere klarhed omkring Socialdemokratiets skiftende holdning til statsborgerskab for mistænkte personer.</t>
+          <t>Der er bekymring over tildelingen af dansk statsborgerskab til personer, vurderet som sikkerhedsrisikoer, som rejser spørgsmål om internationale konventioners fortolkning og Danmarks integration og statsborgerskabspolitik.</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Dansk Folkeparti afviser et lovforslag om statsborgerskab for 1.109 personer, da de mener, det vil underminerer integration og ligebehandling, samtidig med at de stiller spørgsmål ved relevansen af oprindelseslandet, når de fastsatte krav for statsborgerskab er opfyldt.</t>
+          <t>Dansk Folkeparti afviser lovforslaget om statsborgerskab med fokus på integration, ligebehandling og krav til ansøgere, samtidig med at de kritiserer lempelser i danskkundskaber og relationer til statsløse konventioner.</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Dansk Folkeparti's politiske holdninger kritiseres for at være problematiske og potentielt diskriminerende over for muslimer og personer med tilknytning til muslimske lande, hvilket rejser spørgsmål om tildeling af dansk statsborgerskab og skaber bekymring for demokratiske værdier i Danmark. Der er også tvivl om partiets klare retningslinjer for statsborgerskab og muligheden for at stille forskellige krav til muslimer sammenlignet med andre grupper.</t>
+          <t>Dansk Folkepartis politik rejser spørgsmål om diskrimination mod muslimer og parallelsamfund i Danmark, samt uklarheder i deres krav til statsborgerskab, hvilket skaber bekymring for demokratiske værdier.</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Flere politiske partier i Danmark diskuterer et lovforslag, der muliggør dansk statsborgerskab for 1.109 personer, samtidig med at der er bekymringer og forslag om strengere krav til ansøgerne, herunder selvforsørgelse og fravær af kriminalitet. Der er en generel enighed om, at statsborgerskab er vigtigt for integration og anerkendelse af individers bidrag til samfundet.</t>
+          <t>Der er bred politisk støtte til et lovforslag om dansk statsborgerskab for 1.109 personer, men samtidig er der bekymringer om kravene og ønsker om strengere regler.</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Der er en afvisning af ændringer i sprog- og selvforsørgelseskrav samt statsborgerskabsprøven, da indvandringen fra ikkevestlige muslimske lande ses som en trussel mod dansk kultur, og der rejses bekymringer om parallelsamfund og integration, hvilket understreger behovet for strengere krav og midlertidig status for flygtninge.</t>
+          <t>Der er en fælles bekymring for indvandringens indvirkning på dansk kultur og samhørighed, samt en opfordring til at begrænse indvandringen fra ikkevestlige lande og stille krav til statsborgerskab for at sikre integration.</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Debatten om tildeling af dansk statsborgerskab fokuserer på glæden ved, at mange opnår statsborgerskab, samtidig med at der rejses alvorlige bekymringer over sikkerhedsrisici forbundet med at inkludere personer, der vurderes som trusler mod rigets sikkerhed, i lovforslag. Der er også kritik af politiske partiers håndtering af fortrolige oplysninger og deres konsekvenser for national sikkerhed samt spørgsmål om, hvordan disse situationer relaterer sig til grundlovens rammer for ytringsfrihed.</t>
+          <t>Debatten om dansk statsborgerskab fremhæver både glæden ved indfødsret for mange borgere og bekymringer over tildele statsborgerskab til personer vurderet som sikkerhedsrisikoer, hvilket rejser spørgsmål om ansvar, sikkerhed og politiske beslutninger.</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Ordføreren er blevet kritiseret for manglende offentliggørelse af dokumenter vedrørende fortrolige oplysninger, hvilket rejser spørgsmål om håndtering af information fra PET i forbindelse med tildeling af statsborgerskab, mens der er intern uenighed blandt Socialdemokratiet om, hvorvidt PET's rådgivning skal påvirke denne proces. Samtidig understreges vigtigheden af, at personer anses som uskyldige, indtil det modsatte er bevist, og at offentliggørelse af følsomme oplysninger kan have alvorlige konsekvenser.</t>
+          <t>Der er en debat om offentliggørelse af fortrolige oplysninger og håndtering af statsborgerskab, hvor forskellige synspunkter inden for Socialdemokratiet og spørgsmål om lovgivningens rammer spiller en central rolle.</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Debatten om lovforslaget om statsborgerskab afslører en splittelse mellem Venstre og Dansk Folkeparti, præget af bekymringer om procedure, fortrolighed og sikkerhed, samt kritik af, hvordan offentliggørelse af fortrolige oplysninger kan påvirke ansøgere, der har bidraget positivt til samfundet. Der er også en opfordring til åben diskussion om konventioner og en vurdering af, hvordan stigende sagsbehandlingstider kan påvirke antallet af tildelte statsborgerskaber.</t>
+          <t>Debatten om lovforslaget om statsborgerskab viser en splittelse mellem partierne, hvor fokus er på procedure og jura, samtidig med at der er bekymringer om behandlingen af fortrolige oplysninger og behandlingen af ansøgninger.</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Der rejses spørgsmål om regeringens politik vedrørende tildeling af statsborgerskab og håndtering af statsborgerskab for personer i PET's søgelys, herunder kritik af lange sagsbehandlingstider og faldet i antallet af nye statsborgere, samt en debat om inkonsekvenser i støtte til PET fra Enhedslisten. Der er også en understregning af, at der ikke er planer om at ændre de nuværende principper for statsborgerskab.</t>
+          <t>Der er en debat om statsløse personer, flygtninge- og integrationslovgivning samt tildeling af statsborgerskab i Danmark, hvor regeringens nuværende politik og tidligere fejl, herunder sagsbehandlingstider og PET's rolle, drøftes.</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Der er blevet givet mange dispensationer til ansøgere om dansk statsborgerskab, hvilket har medført lempelser af kravene, herunder sprogkrav, hvilket Dansk Folkeparti er imod og mener bør strammes.</t>
+          <t>Der er blevet givet mange dispensationer til dansk statsborgerskab, hvilket har ført til lempelser af kravene, men Dansk Folkeparti ønsker strammere krav.</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Tildelingen af dansk statsborgerskab bør fokusere mere på integration og sprogkundskaber for at sikre, at nyankomne kan blive en del af det danske samfund, samtidig med at der skal sikres en ordentlig behandling af dem, der opfylder kravene.</t>
+          <t>Tildelingen af dansk statsborgerskab bør fokusere mere på integration og sprogkundskaber for at sikre, at nyankomne bedre kan blive en del af det danske samfund.</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Lovforslaget er problematisk, da det kombinerer tildeling af dansk statsborgerskab til både berettigede personer og dem, der får det via dispensationsansøgninger, men Liberal Alliance vælger at støtte det, da størstedelen af ansøgningerne overholder retningslinjerne.</t>
+          <t>Lovforslaget skaber bekymring ved at blande berettigede statsborgerskabsansøgere med dem, der får dispensation, men Liberal Alliance vælger at støtte det på grund af overholdelse af retningslinjerne.</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Lovforslaget om tildeling af dansk statsborgerskab får positiv støtte fra den konservative side, som understreger betydningen af statsborgerskabsdagen som en vigtig tradition for at byde nye borgere velkommen.</t>
+          <t>Lovforslaget om dansk statsborgerskab får positiv støtte fra konservative, der værdsætter statsborgerskabsdagen som en vigtig tradition.</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>679 voksne og ca. 425 børn opnår dansk statsborgerskab ved at opfylde specifikke krav, og det er vigtigt at anerkende de unikke udfordringer, som mange statsborgerskabssøgere, herunder krigsofre, har mødt, da de fortjener tryghed og rettigheder i Danmark.</t>
+          <t>679 voksne og ca. 425 børn opnår dansk statsborgerskab, hvilket indebærer opfyldelse af betingelser og anerkendelse af deres unikke baggrunde og udfordringer.</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>679 voksne og deres børn har fået dansk statsborgerskab, men processen er lang og besværlig med lange sagsbehandlingstider og høje krav, på trods af mere humane regler for særlige grupper.</t>
+          <t>Dagen fejres af 679 nye danske statsborgere, men processen for at opnå statsborgerskab er lang og kompliceret trods forbedringer for særlige grupper.</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Velkomsten af nye statsborgere til det danske fællesskab er en betydningsfuld begivenhed, som understøttes af Folketinget, især med hensyn til muligheden for at have statsborgerskab i flere lande.</t>
+          <t>Velkomsten af nye statsborgere til det danske fællesskab og anerkendelsen af muligheden for statsborgerskab i flere lande er vigtige og glædelige begivenheder.</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Debatten om indfødsretslovforslaget centrerer sig om stramninger ved tildeling af statsborgerskab, politisk anstændighed, og spørgsmålet om, hvordan man retfærdigt kan behandle ansøgninger, især for børn født i Danmark og personer med psykologiske udfordringer. Der rejses også bekymringer om konsekvenserne af politiske holdninger og ytringer på statsborgerskab, samt behovet for generelle regler og realisme i sprogkravene.</t>
+          <t>Debatten om indfødsretslovforslaget centrerer sig om principielle spørgsmål ved tildeling af statsborgerskab, hvor der er fokus på politisk anstændighed, integration af ansøgere, samt nødvendigheden af at respektere tidligere aftaler og sikre ensartet behandling.</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Der er fokus på vigtigheden af, at ansøgere til dansk statsborgerskab viser loyalitet over for demokratiet og ikke tilhører totalitære ideologier, samt behovet for at skelne mellem forskellige grupper i vurderingen af ansøgninger. Desuden diskuteres det politiske ansvar i beslutningsprocessen for tildeling af statsborgerskab samt muligheden for dispensation baseret på individuelle forhold.</t>
+          <t>Der er behov for en grundig vurdering af ansøgere om dansk statsborgerskab, der inkluderer loyalitet over for demokratiet og skelnen mellem forskellige holdninger samt en politisk beslutningsproces fremfor medicinske vurderinger.</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Debatten om dansk statsborgerskab centrerer sig om håndteringen af ansøgninger, politiske ytringer og de krav, der stilles til ansøgere, herunder respekt for demokratiet, sprogkrav og selvforsørgelse, hvilket har ført til bekymringer om retssikkerhed og konsekvenserne af politiske beslutninger. Der er også kritik af, at politiske holdninger kan påvirke tildelingen af statsborgerskab, hvilket rejser spørgsmål om ytringsfrihed og ensartede retningslinjer for ansøgninger.</t>
+          <t>Debatten om dansk statsborgerskab centrerer sig om krav til sprog, selvforsørgelse, politiske ytringer og retssikkerhed, hvor der er bekymringer om, hvordan disse faktorer påvirker tildelingen af statsborgerskab og integration i samfundet.</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Fru Lotte Rod fra Radikale Venstre bliver gentagne gange nævnt i teksten.</t>
+          <t>Fru Lotte Rod nævnes gentagne gange i teksten.</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Dansk Folkeparti mener, at tildelingen af dansk statsborgerskab bør tage hensyn til Danmarks fremtid og sammenhængskraft, og de kritiserer tildelingen af for mange statsborgerskaber for at svække landets værdier og folkelige sammenhængskraft.</t>
+          <t>Dansk Folkeparti mener, at tildelingen af dansk statsborgerskab bør prioritere Danmarks fremtid og sammenhængskraft.</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Der er en enighed om, at unødvendige forhindringer for dansk statsborgerskab skader samfundets sammenhængskraft, selvom tildelingen af statsborgerskab til mange personer er en positiv udvikling.</t>
+          <t>Der er enighed om, at unødvendige forhindringer i indfødsretssager skader samfundets sammenhængskraft, mens det er positivt at bevilge statsborgerskab til mange individer.</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Der kritiseres en tidligere praksis for utilstrækkelig sagsbehandling af ansøgninger, hvilket har skabt behov for klare retningslinjer fra Indfødsretsudvalget for at sikre kvalificerede beslutninger om integration og reducere politisk indblanding, især for sårbare grupper som mennesker med posttraumatisk stress.</t>
+          <t>Der er behov for alvorlige ændringer i sagsbehandlingen af ansøgninger, herunder tydeligere retningslinjer, for at sikre kvalificerede beslutninger om integration og tage hensyn til menneskers liv.</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Afstemningen om flere ændringsforslag har resulteret i både vedtagelse og forkastelse af forskellige forslag, hvor flertallet af udvalget, med undtagelse af DF, har tiltrådt de fleste ændringer, samtidig med at der er blevet foreslået at gå direkte til tredje behandling af lovforslaget uden fornyet udvalgsbehandling. Diskussionen omhandlende retningslinjer for indfødsret og politisk vurdering af dispensation fremhæver behovet for fleksibilitet i tildelingen af statsborgerskab.</t>
+          <t>Der er afstemninger om forskellige ændringsforslag, hvor flertallet støtter flere forslag, mens nogle enkelte forslag bliver forkastet.</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Der udtrykkes stolthed over nye danske statsborgere og anerkendelse af deres udfordrende rejse, samtidig med bekymringer om retssikkerhed i dispensationsbehandling og krav til sprog, selvforsørgelse og kriminalitet, som er centrale emner i lovforslaget fra Det Konservative Folkeparti for at forbedre statsborgerskabsprocessen.</t>
+          <t>Der er stolthed over nye danske statsborgere og anerkendelse af deres udfordringer, samtidig med bekymringer om retssikkerhed og krav til integration, herunder sprog og selvforsørgelse.</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Tillykke til de 3.185 nye danske statsborgere, men der er bekymringer om retssikkerheden for dem, der ikke er omfattet af lovforslaget, især ansøgere med handicap og personer med kortvarig social ydelse.</t>
+          <t>Tillykke til de nye danskere, men bekymringer om retssikkerhed for udelukkede ansøgere er rejst.</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>For at opnå dansk statsborgerskab skal man opfylde strenge krav, herunder danskkundskaber og kendskab til Danmark, hvilket understreges af den kommende tildeling af statsborgerskab til over 4.000 personer.</t>
+          <t>At blive dansk statsborger kræver opfyldelse af strenge krav og anses som et stort privilegium, hvilket fremhæves af tildelingen af statsborgerskab til mange voksne og børn.</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Lovforslaget L 71 muliggør, at 3.185 personer kan få dansk statsborgerskab, hvilket anerkender deres bidrag til samfundet og understreger vigtigheden af krav som selvforsørgelse og sprogkundskaber, mens Socialdemokratiet opfordrer dem til aktivt at deltage i samfundet.</t>
+          <t>Lovforslaget L 71 muliggør, at 3.185 nye danskere bliver statsborgere, hvilket anerkender deres bidrag og opfordrer til aktiv samfundsdeltagelse.</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Der er vedtaget flere ændringsforslag vedrørende udlændinge- og integrationsministerens betænkning, og der rejses spørgsmål om kriterier for dansk statsborgerskab samt Dansk Folkepartis engagement i disse initiativer, hvilket skaber behov for politisk stabilitet og klarhed om aftalerne.</t>
+          <t>Der er enighed om at fastsætte kriterier for at reducere antallet af personer, der opnår dansk statsborgerskab, samtidig med at der diskuteres politisk stabilitet og sagsbehandlingstider i asyl- og statsborgerskabsprocessen.</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Liberal Alliance ser dansk statsborgerskab som et privilegium, der skal være en udfordring at opnå, og betoner vigtigheden af, at nye danskere tilslutter sig danske værdier og deltager i demokratiet, samtidig med at der er bekymringer om antallet af asylansøgere og behovet for bedre integration. Debatten om lovforslaget, der giver statsborgerskab til 2.139 personer, understreger også behovet for at differentiere mellem asylansøgere og kvalificerede statsborgerskabssøgere samt kritiserer nuværende sagsbehandlingsmetoder.</t>
+          <t>Debatten om dansk statsborgerskab fokuserer på at skærpe betingelserne og anerkende nye danskeres ønske om integration, samtidig med at der er bekymringer om indvandringens indflydelse på Danmarks fremtid.</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Lovforslaget om tildeling af dansk statsborgerskab til 2.139 borgere fremhæver vigtigheden af aktiv deltagelse i samfundet og respekten for danske værdier, mens Dansk Folkeparti kritiserer forslaget og advarer mod konsekvenserne af at give statsborgerskab til flygtninge. Talen anerkender de nye statsborgeres bidrag til Danmark og understreger betydningen af lighed, demokrati og integration.</t>
+          <t>Lovforslaget om tildeling af dansk statsborgerskab til 2.139 borgere fremhæver vigtigheden af aktiv samfundsdeltagelse, respekt for danske værdier og anerkendelse af nye statsborgere som ligestillede medlemmer af det danske samfund.</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Der er behov for et mere retfærdigt og gennemsigtigt system for sagsbehandling af danske statsborgerskaber, da nogle nye statsborgere og efterkommere stadig føler sig afvist i samfundet.</t>
+          <t>Der er behov for et mere retfærdigt og gennemsigtigt system for sagsbehandlingen af ansøgninger om dansk statsborgerskab, da mange efterkommere stadig føler sig afvist i samfundet.</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Lovforslaget om tildeling af dansk statsborgerskab til 1.225 voksne og ca. 159 børn fremhæver vigtigheden af aktiv deltagelse i det danske demokrati, mens Socialdemokratiet støtter det men kritiserer sagsbehandlingstiderne; samtidig viser Alternativets interesse for regulering af kødforbrug en opmærksomhed på befolkningens kostvaner.</t>
+          <t>Lovforslaget om dansk statsborgerskab understreger vigtigheden af aktiv deltagelse i demokratiet og anerkender grundlæggende værdier, samtidig med at der er politisk støtte og bekymringer om sagsbehandlingstider.</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Der er blevet tildelt mange danske statsborgerskaber, men integrationsvanskeligheder har ført til krav om begrænsninger, mens Enhedslisten fremhæver vigtigheden af statsborgerskab og ønsker en lettere proces, især for børn, samtidig med at der stilles spørgsmål ved kravene og den reelle integration af de nye statsborgere.</t>
+          <t>Der er bekymring om integrationen af nye danske statsborgere, hvilket har ført til krav om strammere regler og en debat om, hvordan statsborgerskab tildeles.</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Alternativet byder de 1.225 nye danske statsborgere velkommen og fremhæver vigtigheden af deres deltagelse i samfundet samt behovet for en imødekommende tilgang fra danske institutioner.</t>
+          <t>Alternativet byder de nye danske statsborgere velkommen og opfordrer til aktiv deltagelse i samfundet.</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Statsborgerskab er afgørende for integration og anerkendelse af personer i Danmark, da det giver dem mulighed for aktivt at deltage i samfundet og øger deres følelse af tilhørsforhold, samtidig med at der er et ønske om at lette betingelserne for at opnå det.</t>
+          <t>Statsborgerskab er essentielt for integration og anerkendelse af individer i Danmark, da det muliggør fuld deltagelse i samfundet og styrker tilhørsforholdet.</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>DF argumenterer for strammere betingelser for statsborgerskab for at beskytte dansk kultur og samfund, mens der fejres 1.953 voksne og 472 børn, der nu får dansk statsborgerskab efter at have opfyldt krav om integration og respekt for demokratiske værdier. Der er en ambivalens omkring statsborgerskab, hvor man ønsker at støtte loyale bidragydere, men samtidig ekskludere dem, der ikke deler danske værdier.</t>
+          <t>Der er en ambivalens omkring tildeling af dansk statsborgerskab, hvor der ønskes strammere betingelser for at sikre integration og støtte til dem, der respekterer danske værdier, samtidig med at man undgår at inkludere dem, der modsætter sig demokratiet.</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Venstre anerkender betydningen af at tildele dansk statsborgerskab til voksne og børn, men kritiseres for en afvisende tone over for dem, der har kæmpet for det, samtidig med at der stilles spørgsmål ved partiets holdning til dobbelt statsborgerskab og loyalitet over for flere lande.</t>
+          <t>Venstre anerkender betydningen af statsborgerskab for voksne og børn, men der er bekymringer om partiets tilgang til dobbelt statsborgerskab og loyalitet over for flere lande.</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Der kritiseres en lemfældig tildeling af indfødsret i Danmark, og der argumenteres for strenge betingelser samt en opdeling mellem vestlige og ikke-vestlige indvandrere, mens der samtidig anerkendes nye danskere for deres indsats og opfordres til aktivt at bidrage til samfundet. Lovforslaget L 41, der bygger på tidligere politiske aftaler, stemmes der for trods ønsket om strammere krav.</t>
+          <t>Der er bekymring om indfødsret i Danmark, som bør tildeles under strenge betingelser for at sikre bedre integration og samfundsloyalitet, samtidig med at der anerkendes indsatsen fra nye statsborgere.</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Optagelsen af 3.500 ansøgere til statsborgerskab i Danmark markerer en milepæl, men adgangen er stadig præget af strenge krav og bureaukrati, hvilket især påvirker sårbare grupper. Enhedslisten ønsker at lette adgangen til statsborgerskab og kritiserer den nuværende udlændingelov, mens der fremføres forslag om at revidere reglerne for indfødsret.</t>
+          <t>Der er behov for at lette adgangen til statsborgerskab i Danmark, da nuværende strenge krav og bureaukrati gør det svært for mange, især sårbare grupper, at opnå dette.</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Statsborgerskab i Danmark kræver identifikation med dansk kultur, sprogbeherskelse og samfundsengagement, hvilket fører til en debat om klare krav og kontrol i statsborgerskabsprocessen, samt bekymringer omkring kulturelle og religiøse tilpasninger blandt ansøgere. Lovforslaget L 41 vækker blandede følelser, da der er både glæde over nye statsborgere og ønsker om strammere screening og kriterier.</t>
+          <t>Debatten om statsborgerskab i Danmark fokuserer på krav om dansk identitet, sprogbeherskelse og samfundsengagement, samt nødvendigheden af klare kriterier og screeningsprocesser for ansøgere.</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Teksten kritiserer udlændingeloven fra 1983 og diskuterer lovforslag L 41 om statsborgerskab, hvor Dansk Folkeparti stemmer nej for at beskytte danske værdier, mens der stilles spørgsmål ved andre partiers holdninger og fokus på individers bidrag til samfundet. Der er en generel bekymring for Danmarks tryghed og sikkerhed i forhold til indvandreres integration og bidrag.</t>
+          <t>Der er en fælles bekymring for, hvordan udlændingeloven og statsborgerskabsforslag påvirker Danmarks sikkerhed og samfundsmæssige bidrag fra udlændinge.</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Enhedslisten kritiserer de strenge regler for statsborgerskab og opfordrer til mere gennemsigtighed, mens Nye Borgerlige og Konservative Folkeparti ønsker højere krav og er skeptiske over for massetildeling af statsborgerskaber, især til kriminelle. Der er en generel opfordring til at sikre retssikkerhed og ligebehandling i statsborgerskabsprocessen, samtidig med at der udtrykkes støtte til nye danskere og anerkendelse af sydslesvigerne.</t>
+          <t>Der er en bred debat om tildeling af dansk statsborgerskab, hvor flere partier anerkender glæden ved nye statsborgere, men kritiserer strenge regler og politiske beslutninger, mens andre ønsker at beskytte statsborgerskabet som en værdifuld gave.</t>
         </is>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Teksten omhandler anerkendelsen af 2.944 nye danskere og de krav, der stilles til deres forpligtelse overfor det danske samfund, samtidig med at der kritiseres politiske partier som Socialdemokratiet og Dansk Folkeparti for deres håndtering af statsborgerskab og kriminalitet. Der er en opfordring til at stramme reglerne omkring fratagelse af statsborgerskab ved alvorlig kriminalitet, hvilket Venstre har taget initiativ til.</t>
+          <t>Nye danskere anerkendes for deres bidrag, mens der stilles krav om forpligtelse til det danske samfund, samtidig med politisk debat om statsborgerskab og stramning af regler mod kriminalitet.</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Afstemninger om ændringsforslag vedrørende dansk statsborgerskab har medført forkastelse af flere forslag fra DF og NB, mens der er opbakning til andre forslag fra et flertal af partier. Der er desuden bekymringer over ændringer i reglerne for statsborgerskab, nødvendigheden af stabilitet i udlændingeområdet, og behovet for at revurdere integrationskravene og sikre retssikkerhed for ansøgere.</t>
+          <t>Debatten om dansk statsborgerskab centrerer sig om kravene til ansøgere, retssikkerhed, integration, og politiske værdier, med fokus på at sikre, at kun velintegrerede personer får statsborgerskab, mens der er bekymringer over ændringer i reglerne og politisk samarbejde.</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>De Konservative og Dansk Folkeparti udtrykker bekymringer om tildeling af dansk statsborgerskab, især i forhold til kriminelle udlændinge og integration af personer fra ikke-vestlige kulturer, mens der er usikkerhed om partiernes fremtidige retninger og konsekvenserne af deres politiske aftaler. Der efterlyses en mere individuel vurdering af ansøgere og strammere regler for statsborgerskab, især med fokus på kulturelle forskelle.</t>
+          <t>Der er en politisk debat om indfødsret og statsborgerskab i Danmark, hvor partierne udtrykker bekymring for integration, krav til ansøgere og prioritering af danske værdier, især i relation til personer med muslimsk baggrund.</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Enhedslisten anerkender optagelsen af nye statsborgere under midlertidige ændringer i håndtrykskravet, men kritiserer samtidig den hårde praksis over for ansøgere, især dem med funktionsnedsættelser, samt behovet for reformer i statsborgerskabsreglerne og modstanden mod arrangerede ægteskaber. Der er en bred debat om kriterierne for dansk statsborgerskab, som involverer forskellige politiske holdninger og krav om at respektere individets rettigheder uafhængigt af personlig tro eller overbevisning.</t>
+          <t>Der er en fælles anerkendelse af behovet for at revidere reglerne for dansk statsborgerskab, med fokus på retfærdighed, lighed og respekt for ansøgeres rettigheder, samtidig med at der tages hensyn til sundhedsanbefalinger.</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Debatten om tildeling af dansk statsborgerskab centrerer sig om kravene til ansøgere, herunder håndtryk ved grundlovsceremonien og strammere regler for kriminelle, samt politiske uenigheder mellem partierne om ændringer i udlændingepolitikken, især i lyset af covid-19 og eksisterende aftaler. Der er også bekymring over, hvordan ændringer vil påvirke allerede ventende ansøgere og den generelle respekt for danske værdier.</t>
+          <t>Debatten om dansk statsborgerskab fokuserer på kravene til ansøgere, herunder håndtryk og kriminel baggrund, samt den politiske konflikt mellem partierne om udlændingepolitikken og tildeling af statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Teksten handler om tildelingen af dansk statsborgerskab, hvor der udtrykkes støtte til krav om håndtryk som en del af indfødsretsprocessen og en opfordring til mere nuancerede vurderinger af ansøgninger, samtidig med at der kritiseres venstrefløjen for deres tilgang til emnet og bekymringer over indvandreres kriminalitet. Der er også en anerkendelse af de nye statsborgere og deres bidrag til samfundets værdier som demokrati og ligestilling.</t>
+          <t>Tillykke til nye danskere med statsborgerskab, hvor fokus er på samfundsengagement og tilpasning, samtidig med bekymringer om lovgivning, herunder håndtrykskravet og indvandreres kriminalitet.</t>
         </is>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Indfødsretsudvalget spiller en central rolle i Danmarks fremtid og det politiske landskab, hvor der er behov for en balance mellem strenge krav til statsborgerskab og respekt for demokratiske processer, samt en debat om, hvordan indfødsret skal forstås som en gave fra det danske folk fremfor en rettighed. Diskussionen berører også emner som håndtrykskrav, bekymringer om kriminelle udlændinge, og forholdet mellem den danske kultur og islam.</t>
+          <t>Debatten om indfødsret i Danmark fokuserer på kravene til statsborgerskab, fortrolighed i udvalgsarbejde, og hvordan forskellige grupper opfattes i forhold til tildeling af dansk statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Lovforslaget om massetildeling af danske statsborgerskaber møder kritik for at blande kvalificerede ansøgere med mindre kvalificerede, især fra muslimske lande, hvilket har ført til opfordringer om strengere udvælgelseskrav og klare regler for alvorlig kriminalitet, mens der er enighed om, at børn født eller opvokset i Danmark bør have lettere adgang til statsborgerskab. Derudover er der indgået aftaler om gældstyper, der påvirker muligheden for at opnå statsborgerskab, mens kun få partier ønsker grundlæggende ændringer i den nuværende ordning.</t>
+          <t>Lovforslaget om massetildeling af danske statsborgerskaber kritiseres for at blande kvalificerede ansøgere med mindre kvalificerede, hvilket rejser behovet for strengere udvælgelse og klare regler for statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Der er omfattende kritik af udlændinge- og integrationsministerens manglende vilje til at besvare spørgsmål om tildeling af dansk statsborgerskab, hvilket underminerer Folketingets beslutningsproces og rejser bekymringer om gennemsigtighed og retfærdighed, især i forhold til ansøgere med kriminel baggrund. Debatten fokuserer på strammere krav til statsborgerskab, nødvendigheden af samarbejde med Indfødsretsudvalget og de potentielle konsekvenser af ministerens handlinger for både ansøgere og samfundet som helhed.</t>
+          <t>Debatten om tildeling af dansk statsborgerskab er præget af utilfredshed med ministerens manglende gennemsigtighed og samarbejde, hvilket skaber bekymringer om retfærdighed, strammere krav og mulige konsekvenser for personer med kriminel baggrund.</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Teksten diskuterer kravene for dansk statsborgerskab, herunder sprogkundskaber, lovlydighed og selvforsørgelse, samt politiske holdninger til reformer og opstramninger relateret til kriminalitet, værdier og diskrimination i ansøgningsprocessen. Der er også bekymringer over manglende indsigt i lovgivningen og behovet for objektive kriterier i behandlingen af ansøgninger.</t>
+          <t>Debatten om dansk statsborgerskab fokuserer på krav som sprogkundskaber, lovlydighed og selvforsørgelse samt bekymringer om kriminalitet og integration, hvilket fører til forslag om strammere regler og reformer i behandlingen af ansøgninger.</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Statsborgerskab i Danmark er en kompleks proces, der involverer politiske overvejelser og retssikkerhed, hvor partier som Enhedslisten og Radikale Venstre ønsker at sikre klare kriterier og objektiv behandling, mens Dansk Folkeparti ønsker at adskille ansøgere baseret på nationalitet og baggrund. Der er bekymringer om politisering af statsborgerskabsprocessen og behovet for retfærdighed i behandlingen af ansøgninger.</t>
+          <t>Statsborgerskab i Danmark kræver klare kriterier og en retfærdig proces, samtidig med at der er politiske uenigheder om behandling af ansøgere fra forskellige lande.</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Der er behov for reform af strenge regler for dansk statsborgerskab, så mange langvarige beboere kan opnå fulde borgerrettigheder, mens debatten fokuserer på nye krav til statsborgerskab og imødekommelse af covid-19-situationen. Enhedslisten støtter de nye statsborgere, mens Konservative afviser lovforslaget på grund af skærpede krav, der træder i kraft senere.</t>
+          <t>Der er behov for reform af reglerne for dansk statsborgerskab for at inkludere flere, mens debatten om indfødsretslovforslaget omhandler både tildeling af statsborgerskab og nye skærpede krav.</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Der har været en afstemning om ændringsforslag til et lovforslag, hvor forslagene blev forkastet eller vedtaget, og der stilles spørgsmålstegn ved procedurerne omkring skattepligt og indfødsret i relation til Grundloven.</t>
+          <t>Der er blevet stemt om forskellige ændringsforslag til et lovforslag, hvor et flertal har vedtaget flere ændringer, mens der også er rejst bekymringer om lovgivningsprocessen og grundlovens bestemmelser vedrørende statsborgerskab og skat.</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Der er et behov for at anerkende og byde borgere velkommen, der opfylder betingelserne for dansk statsborgerskab, men der er samtidig bekymringer om kontrol med ansøgere fra muslimske lande og inkonsistens i håndteringen af statsborgerskab, hvilket kræver en differentieret politik for at sikre danske værdier og retsstatens principper.</t>
+          <t>Der er behov for at anerkende og byde velkommen til borgere, der opfylder betingelserne for dansk statsborgerskab, samtidig med at der stilles krav om respekt for danske værdier og en differentieret tilgang til ansøgere baseret på oprindelsesland.</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Tildelingen af danske statsborgerskaber kritiseres for manglende ansvarlighed, og der er krav om strammere regler fra partier som Nye Borgerlige og Dansk Folkeparti, der fokuserer på at sikre positive bidrag til samfundet og beskytte sammenhængskraften, mens nytilkomne statsborgere undergår en krævende proces for at integrere sig og værdsætte danske værdier.</t>
+          <t>Der er en fælles bekymring blandt partierne om ansvarligheden ved tildeling af danske statsborgerskaber og betydningen af, at ansøgerne bidrager positivt til samfundet.</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Der er en bred opbakning til lovforslaget om indfødsret, som anerkender det engagement, mange ansøgere har vist for at blive en del af det danske samfund, men der er samtidig bekymringer om retssikkerheden, diskrimination i ansøgningsprocessen og behovet for strenge kriterier for at opnå statsborgerskab. Diskussionen involverer også forslag til forbedringer i sagsbehandlingen og en balance mellem objektive kriterier og individuel behandling af ansøgninger.</t>
+          <t>Der er en bred enighed blandt partierne om behovet for at forbedre retssikkerheden og proces for dansk statsborgerskab, samtidig med at der understreges vigtigheden af strenge kriterier og engagement i det danske samfund.</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Debatten om dansk statsborgerskab centrerer sig om kravene til indfødsret, håndtering af grove forbrydelser, og hvordan forskellige politiske partier forholder sig til fratagelse af statsborgerskab, samtidig med at der er fokus på at sikre retfærdighed for ofre og opretholde internationale konventioner. Der stilles spørgsmål ved, hvordan man kan balancere integration, kriminalitetsforebyggelse og beskyttelse af samfundets interesser.</t>
+          <t>Debatten om dansk statsborgerskab fokuserer på krav til integration, håndtering af grov kriminalitet og beskyttelse af ofre, samtidig med at der stilles spørgsmål til de forskellige politiske partiers holdninger til statsborgerskabsfratagelse og internationale konventioner.</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Debatten om dansk statsborgerskab fokuserer på behovet for reformer af tildelingsprocessen, herunder klare kriterier og individuel vurdering, for at sikre, at statsborgerskabet værdsættes og kun gives til dem, der aktivt bidrager til samfundet, samtidig med at der udtrykkes bekymringer om potentielle sociale konsekvenser af den nuværende praksis. Både støtte og modstand til ændringerne belyser uenigheder om udlændingepolitik og integration i Danmark.</t>
+          <t>Debatten om dansk statsborgerskab fokuserer på behovet for klare kriterier og individuel vurdering af ansøgere, samtidig med at der udtrykkes bekymring for samfundets sammenhængskraft og retfærdighed i tildelingsprocessen.</t>
         </is>
       </c>
     </row>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Teksten diskuterer problematikker relateret til indfødsret og statsborgerskab i Danmark, herunder misforståelser om kriterierne for statsborgerskab, konsekvenserne af kriminelle handlinger, og behovet for en retfærdig og demokratisk proces, der anerkender rehabilitering og samfundsengagement. Derudover fremhæves vigtigheden af at sikre retssikkerhed for ofre og overholdelse af internationale menneskerettigheder i forbindelse med statsborgerskabsfratagelse.</t>
+          <t>Diskussionen om indfødsret fokuserer på retfærdighed og retssikkerhed for alle borgere, inklusive hvordan tidligere kriminelle kan rehabiliteres og genopnå statsborgerskab, samt vigtigheden af at sikre, at personer med ekstremistiske holdninger ikke får indfødsret.</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Der er bekymringer over den nye indfødsretsaftale, som kan føre til diskrimination og manglende ligestilling, og der er behov for anerkendelse af mangfoldighed og forskellighed i måden, mennesker interagerer på.</t>
+          <t>Der er bekymringer om den nye indfødsretsaftale, da den kan føre til diskrimination og underkende vigtigheden af mangfoldighed og anerkendelse mellem mennesker.</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Massetildelingen af statsborgerskaber kritiseres for at mangle kriterier og resultere i tildelinger til uegnede personer, især fra muslimske lande, mens flere ændringsforslag om ændringer i behandlingen af statsborgerskabsansøgninger bliver forkastet. Der er en opfordring til at forbedre systemet for at sikre, at statsborgerskab tildeles dem, der virkelig fortjener det.</t>
+          <t>Kritikken af massetildelingen af statsborgerskaber fokuserer på manglende kriterier og uigennemsigtighed, hvilket fører til tildeling af statsborgerskab til uegnede personer.</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Som ny ordfører fremhæves betydningen af statsborgerskab som en grundlæggende del af demokratiet, hvor der er både glæde over de nye danskere og bekymring omkring kriminalitet, hvilket fører til forslag om revidering af reglerne og individuelle vurderinger. Der er en opfordring til inklusion og repræsentation, samtidig med kritik af den nuværende håndtryksceremoni for nye statsborgere.</t>
+          <t>Der er en fælles anerkendelse af betydningen af statsborgerskab som en fundamental del af demokratiet, med fokus på ligebehandling, krav om integration og forskellige syn på reglerne for indfødsret.</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Statsborgerskab opfattes som et privilegium, der bør tildeles værdige ansøgere, mens Dansk Folkeparti kritiserer lovforslaget for at inkludere for mange fra MENAPT-lande og frygter islamisering, mens andre fejrer de, der opnår statsborgerskab efter at have gennemgået en krævende proces.</t>
+          <t>Statsborgerskab ses som et privilegium, der bør tildeles værdige ansøgere, hvilket skaber debat om antallet af ansøgere, især fra MENAPT-lande, mens fejringen af de, der opnår dansk statsborgerskab, markerer berigelsen af det danske fællesskab.</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Lovforslaget om tildeling af dansk statsborgerskab møder kritik for utilstrækkelig kontrol med ansøgere, hvilket kan medføre indfødsret til kriminelle, og der er bekymringer om, at den nuværende praksis er ineffektiv og diskriminerende. Der er et fælles ønske om at sikre, at statsborgerskab kun gives til dem, der positivt bidrager til samfundet, samtidig med at der opfordres til en grundig gennemgang af indfødsretsprocessen.</t>
+          <t>Lovforslaget om tildeling af dansk statsborgerskab mødes med kritik for manglende kontrol og sagsbehandling, hvilket rejser bekymringer om sikkerhed, ansvarlighed og integration af både kriminelle og lovlydige individer.</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Statsborgerskab i Danmark ses som en kilde til glæde, sikkerhed og tilhørsforhold, men der er bekymringer om håndtering af udlændinge, der skaber utryghed, samt om tildelingen af statsborgerskaber til personer, hvis værdier ikke harmonerer med danske normer. Der er også en kritisk debat om, hvordan man sikrer, at nye statsborgere anerkender og tilslutter sig de grundlæggende danske værdier.</t>
+          <t>Statsborgerskab i Danmark fremkalder både glæde og bekymringer over integration, værdier og sikkerhed, med opfordringer til en mere restriktiv tilgang til tildeling af statsborgerskaber, især for personer med problematiske holdninger.</t>
         </is>
       </c>
     </row>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Tildeling af dansk statsborgerskab rejser komplekse spørgsmål om krav, demografiske udfordringer og integration, hvor politiske partier som Enhedslisten og Dansk Folkeparti diskuterer nødvendigheden af retfærdige regler og håndtering af sociale problemer forbundet med statsborgerskab, samtidig med at antisemitisme og islamofobi adresseres som centrale samfundsproblemer. Der er en generel bekymring for, hvordan nuværende politikker påvirker Danmarks økonomi, kultur og sammenhængskraft, og behovet for en mere nuanceret tilgang til statsborgerskab og integration er tydelig.</t>
+          <t>Tildeling af dansk statsborgerskab kræver opfyldelse af strenge krav og rejser vigtige spørgsmål om integration, demografiske ændringer og samfundets sammenhængskraft, samtidig med at der er behov for retfærdige regler og anerkendelse af dem, der fortjener det.</t>
         </is>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Flere ændringsforslag fra mindretal, primært fra DF, blev forkastet i afstemninger, mens nogle forslag fra flertallet blev vedtaget, herunder lovforslagets endelige vedtagelse, som nu sendes til statsministeren. Afstemningerne viste en markant overvægt af stemmer imod de fremsatte ændringsforslag fra mindretallene.</t>
+          <t>Flere ændringsforslag er blevet afstemte og forkastet, mens lovforslaget til sidst er blevet vedtaget og sendt til statsministeren.</t>
         </is>
       </c>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Afstemningerne om ændringsforslag fra Dansk Folkeparti og andre mindretal resulterede i, at samtlige forslag blev forkastet, og lovforslaget blev endeligt vedtaget af et flertal. Derudover blev der rejst forslag om anonymisering af ansøgere om dansk statsborgerskab som reaktion på tidligere sager.</t>
+          <t>Alle ændringsforslag fremsat af Dansk Folkeparti (DF) er blevet forkastet, og lovforslaget er vedtaget uden fornyet udvalgsbehandling.</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Debatten om indfødsret i Danmark fokuserer på behovet for en retfærdig og transparent proces, der overholder handicapkonventionen, samtidig med at der er bekymringer om tildeling af statsborgerskab til personer uden tilstrækkelig tilknytning til landet, hvilket rejser spørgsmål om diskrimination og retssikkerhed. Der er også uenighed blandt partierne om kriterierne for statsborgerskab og behovet for at sikre, at ansøgere opfylder de fastsatte krav, herunder respekt for dansk kultur og værdier.</t>
+          <t>Behandlingen af statsborgerskab i Danmark rejser bekymringer om diskrimination, retssikkerhed og overholdelse af internationale konventioner, herunder handicapkonventionen, samtidig med at der er behov for en mere retfærdig og transparent proces for tildeling af statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Dansk Folkeparti kritiserer regeringens tildeling af danske statsborgerskaber til personer, der ikke respekterer danske værdier, og understreger, at statsborgerskab bør gives til dem, der positivt bidrager til samfundet. Der er en opfordring til at stramme kravene for statsborgerskab og en bekymring for, at nuværende politikker kan føre til tildeling af statsborgerskab til personer med ekstreme holdninger.</t>
+          <t>Dansk Folkeparti kritiserer regeringens statsborgerskabspolitik og mener, at tildeling bør baseres på respekt for danske værdier og samfundspositive bidrag.</t>
         </is>
       </c>
     </row>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Kritikken af Folketingets udlændingepolitik fokuserer på massetildeling af statsborgerskaber og manglende anerkendelse af islamiske værdier som en trussel mod demokratiet, samtidig med at der understreges vigtigheden af ytringsfrihed og ligebehandling af ekstremister. Der er behov for en strammere tilgang til integration, hvor danskhed defineres ud fra kultur og værdier, og der stilles spørgsmål ved ansvar og beslutninger fra politikere i forhold til udfordringerne for den vestlige civilisation.</t>
+          <t>Der rejses kritik af Folketingets udlændingepolitik, især vedrørende statsborgerskaber og integration, med fokus på behovet for ytringsfrihed, bekæmpelse af ekstremisme og en grundlæggende debat om danskhed og værdier.</t>
         </is>
       </c>
     </row>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Der er blevet rejst bekymringer omkring ændringer i ansøgernes sammensætning til indfødsret, politikernes tilgang til screening af ansøgere, samt nødvendigheden af at stramme reglerne for tildeling af dansk statsborgerskab, hvilket har skabt politisk debat og uenighed mellem partierne om, hvordan man bedst håndterer disse spørgsmål. Der er også et behov for en grundlæggende diskussion om værdier og ansvar i forbindelse med statsborgerskab, samt en effektiv behandling af indfødsretssager i Folketinget.</t>
+          <t>Der er behov for en grundig politisk debat og stramninger i indfødsretslovgivningen for at sikre, at ansøgere opfylder danske værdier og undgå tildeling af statsborgerskab til personer med kriminel baggrund.</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Debatten om tildeling af dansk statsborgerskab centrerer sig om balancen mellem strenge krav for at sikre respekt for danske værdier og bekymringer om, at nuværende regler kan udelukke værdige ansøgere, samtidig med at der er frygt for, at personer med antidemokratiske holdninger får statsborgerskab. Der er behov for en mere individuel vurdering af ansøgere, samtidig med at der skal tages højde for beskyttelse af grundlæggende frihedsrettigheder.</t>
+          <t>Debatten om dansk statsborgerskab centrerer sig om kravene til ansøgere, bekymringer om tildeling til personer med antidemokratiske holdninger, og behovet for en principiel tilgang, der sikrer, at nye borgere deler danske værdier.</t>
         </is>
       </c>
     </row>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Afstemningerne om ændringsforslag fra et mindretal (DF) resulterede i, at samtlige forslag blev forkastet, mens flere ændringsforslag tiltrådt af et flertal blev vedtaget. Lovforslaget blev endeligt vedtaget efter afstemning, til trods for et forsøg på at afbryde tredje behandling, som også blev forkastet.</t>
+          <t>Flere ændringsforslag fra DF blev forkastet, mens nogle forslag fra et flertal blev vedtaget, før lovforslaget endeligt blev godkendt.</t>
         </is>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Der er omfattende kritik af administrationen af indfødsretsområdet i Danmark, især vedrørende tildeling af statsborgerskab til personer med kriminel baggrund, hvilket skaber bekymring for lovgivningens integritet og befolkningens tillid. Flere partier opfordrer til strengere regler og grundigere kontrol af ansøgernes værdier og tilknytning til danske værdier for at sikre, at statsborgerskab kun gives til dem, der fortjener det.</t>
+          <t>Der er omfattende kritik af den nuværende administration af indfødsretsområdet, især vedrørende tildeling af dansk statsborgerskab til personer med kriminel baggrund, og der er enighed om behovet for strammere regler og bedre kontrol for at genoprette tilliden til systemet.</t>
         </is>
       </c>
     </row>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Teksten omhandler afstemninger og behandling af ændringsforslag vedrørende statsborgerskab i Danmark, hvor Dansk Folkeparti (DF) har fremsat flere forslag, der er blevet forkastet, mens andre forslag fra regeringen er blevet vedtaget. Der er også en diskussion om de politiske konsekvenser af indfødsretspolitikken, herunder anklager om brud på internationale konventioner, samt behovet for individuel vurdering af ansøgere til statsborgerskab.</t>
+          <t>Diskussionen om indfødsret og statsborgerskab i Danmark er præget af afvisning af ændringsforslag fra Dansk Folkeparti, bekymringer om overholdelse af internationale konventioner, og en stram udlændingepolitik, der fokuserer på individuel vurdering af ansøgere.</t>
         </is>
       </c>
     </row>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Debatten om dansk statsborgerskab fokuserer på kravene til ansøgere, herunder sprog og baggrund, samt bekymringer om diskrimination og integration af personer fra MENAPT-lande, mens der samtidig er en efterspørgsel efter mere viden og bedre screeningsmetoder for at sikre, at ansøgere deler samfundets værdier. Der er også kritiske stemmer om den nuværende statsborgerskabspolitik og behovet for en ekspertgruppe til at undersøge disse spørgsmål.</t>
+          <t>Debatten om dansk statsborgerskab fokuserer på sprogkrav, kontrol af ansøgeres baggrund og holdninger, samt behovet for bedre screeningsmetoder og integration af personer uden statsborgerskab.</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Lovforslaget om tildeling af dansk statsborgerskab til cirka 1.100 personer afspejler ændringer i ansøgernes baggrund og strammere indfødsretskrav, hvilket skaber debat blandt partierne om udlændingepolitik, anerkendelse af nye statsborgere samt bekymringer for konventionsbrud og fremtidige stramninger. Der er fokus på nødvendigheden af at sikre, at statsborgerskab tildeles ansvarligt og i overensstemmelse med danske værdier, samtidig med at der stilles krav til ansøgernes integration og tilknytning til landet.</t>
+          <t>Debatten om lovforslaget om statsborgerskab i Danmark fokuserer på anerkendelse af de 1.100 ansøgere, stramme krav til tildeling, politiske uenigheder og bekymringer om integration og sikkerhed.</t>
         </is>
       </c>
     </row>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Kritikken af Folketingets udlændingepolitik fokuserer på befolkningsudskiftning og islamisering, med Borgernes Parti som det eneste, der ønsker at ændre kursen. Der er bekymring for, hvordan stramme indfødsretsregler og remigration vil påvirke både ansøgere og danske borgere, mens der stilles spørgsmål ved de borgerlige partiers evne til at håndtere disse emner effektivt.</t>
+          <t>Der er en udbredt kritik af Folketingets udlændingepolitik med fokus på behovet for ændringer for at håndtere befolkningsudskiftning og bevare dansk kultur, samt en opfordring til politisk handling fra partier som Borgernes Parti og Dansk Folkeparti.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refreshed LLM outputs for LDA analysis with more topics
</commit_message>
<xml_diff>
--- a/output/results_llm_lda_topics.xlsx
+++ b/output/results_llm_lda_topics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Debatten om indfødsret og kravene til udlændinge, der ønsker dansk statsborgerskab, herunder deling af liberale og demokratiske værdier.</t>
+          <t>Der er enighed om behovet for klare og konsekvente regler for tildeling af dansk statsborgerskab og bekymringer over ændringer af betingelserne efter ansøgninger, hvilket underminerer tilliden til systemet. Diskussionen om statsborgerskab omfatter også spørgsmål om diskrimination baseret på oprindelse, økonomiske kriterier og beskyttelse af grundlæggende frihedsrettigheder. Flere partier ønsker at sikre, at borgere, der opfylder kravene, behandles retfærdigt og ikke bliver påvirket af politiske skift eller fordomme.</t>
         </is>
       </c>
     </row>
@@ -461,137 +461,167 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Der er en række ordførere, der skiftes til at tale, og der udveksles korte bemærkninger om tildeling af dansk statsborgerskab, herunder krav til ansøgere og bekymringer om kontrol og værdimæssig tilknytning.</t>
+          <t>At opnå dansk statsborgerskab kræver opfyldelse af strenge krav, herunder sprogkundskaber, selvforsørgelse og kendskab til danske værdier, hvilket anerkendes som et stort privilegium. Fejringen af de nye statsborgere understreger vigtigheden af deres bidrag til samfundet og muligheden for at deltage aktivt i demokratiet. Der er en generel enighed om, at statsborgerskab fremmer integration og tilhørsforhold, samtidig med at der er ønsker om at lette betingelserne for at gøre det lettere for flere at blive en del af det danske fællesskab.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fælles emne for alle nævnte personer er deres tilstedeværelse eller omtale i en given sammenhæng.</t>
+          <t>Der anerkendes udfordringer forbundet med islamisme og sharialov i visse ghettoer, samt problemer relateret til ikkevestlig indvandring.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Afstemninger om en række ændringsforslag er gennemført, hvor de fleste forslag er blevet forkastet, mens nogle er blevet vedtaget, og lovforslaget vil gå direkte til tredje behandling uden fornyet udvalgsbehandling.</t>
+          <t>Der er behov for, at politikere træffer beslutninger baseret på deres overbevisninger for at sikre Danmarks fremtid og velfærd. Regeringen anerkender forskellige synspunkter og har oprettet en ekspertgruppe for at forbedre borgerbehandlingen, men der er bekymringer om, at sindelagssamtaler kan overtræde retsstatsprincipperne. Der appelleres til ministeren om at sikre, at disse principper respekteres i statsborgerskabsansøgninger.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Der er enighed om vigtigheden af korrekt behandling af statsborgerskabsansøgninger og bekymring for ekstremisme, mens der også er kritik af ministerens håndtering og partipolitik i forhold til indfødsret.</t>
+          <t>Indlægget kritiserer Hr. Jesper Langballes udtalelser som perfide og faktuelt mangelfulde, samtidig med at der påpeges, at direkte tiltale ikke må anvendes i debatten.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tildelingen af dansk statsborgerskab til nye borgere understreger vigtigheden af at opfylde strenge krav som sprogkundskaber, beskæftigelse og respekt for danske værdier, og det betragtes som en anerkendelse af deres bidrag til samfundet.</t>
+          <t>Der er behov for at nedsætte en ekspertgruppe for at opnå resultater, men der er usikkerhed om tidshorisonten. Der søges klarhed over Venstres støtte til den tidligere beslutning om en undersøgelseskommission.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Debatten om indvandring og tildeling af statsborgerskaber i Danmark centrerer sig om bekymringer om demografiske ændringer, integration og kulturel sammenhængskraft, især i relation til personer fra ikkevestlige muslimske lande.</t>
+          <t>Der afholdes en række taler og bemærkninger fra forskellige ordførere i Folketinget, hvor der udveksles synspunkter om udlændingepolitik, kontrol af ansøgere til statsborgerskab og politiske holdninger. Flere parter udtrykker bekymringer over håndteringen af emner såsom kriminalitet og integration, samt behovet for klarhed og ansvarlighed i lovgivningen. Der er også et fokus på samarbejde mellem partierne i den politiske debat.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Der diskuteres stramninger af reglerne for indfødsret og håndhævelsen af disse, herunder spørgsmålet om personer med karensbetingende handlinger.</t>
+          <t>Der er en stigende politisk debat om indfødsret i Danmark, med fokus på at sikre, at statsborgerskab kun tildeles personer, der har vist loyalitet og tilknytning til landet. Der er bekymring over tildelingen af statsborgerskab til personer med kriminel baggrund og et ønske om strammere kriterier og individuel vurdering af ansøgere. Partier som Dansk Folkeparti presser på for at ændre procedurerne, hvilket skaber en kompleks diskussion om balance mellem integration, sikkerhed og danske værdier.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Forhandlingen fokuserer på ændringsforslagene og afsluttes med afstemninger, hvor der ikke er nogen, der ønsker at udtale sig.</t>
+          <t>Der har været en række afstemninger om forskellige ændringsforslag, hvor mange blev forkastet med stor margin. Lovforslaget er blevet vedtaget til direkte behandling uden fornyet udvalgsbehandling, og der er flere ændringsforslag, der er blevet betragtet som vedtaget uden afstemning, når ingen har gjort indsigelse. Generelt set har ændringsforslag fra mindretal, især fra DF, ofte ikke fået støtte fra flertallet.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Fokus på Fru Marie Krarup, Fru Astrid Krag og Fru Ulla Sandbæk samt ministeren.</t>
+          <t>Der er en fælles opfattelse af, at Socialdemokratiet lider under utilstrækkelig intern kommunikation.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Der er fokus på vigtigheden af ligestilling, sprogkrav og respektfuld kommunikation i den politiske debat, samtidig med at der stilles spørgsmål ved håndtryk som en symbolsk handling i relation til køn.</t>
+          <t>Der er enighed blandt partierne om at stramme reglerne for dansk statsborgerskab, herunder krav om, at ansøgere skal dele grundlæggende demokratiske værdier og udelukkelse af personer med kriminel baggrund. Liberal Alliance og andre partier understreger behovet for at håndhæve disse stramninger og prioritere kvalificerede ansøgere.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Høje boglige krav i danske frisøruddannelser kan være en hindring for indvandrere, der ønsker at blive selvforsørgende.</t>
+          <t>Der er en igangværende debat om statsborgerskabslovgivning, hvor forskellige partier stiller spørgsmålstegn ved hinandens holdninger og forslag, herunder håndtering af statsløse personer og krav til ansøgere om statsborgerskab. Der er bekymring for, at massetildeling af statsborgerskaber uden tilstrækkelig kontrol kan have negative konsekvenser for samfundet, samtidig med at der er behov for at balancere demokratiske værdier med sikkerhed og integration. Diskussionen omfatter også hvordan kriminalitet påvirker tildeling af statsborgerskab og hvordan forskellige partier forholder sig til dette emne.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Der er behov for en kritisk debat om tildeling af dansk statsborgerskab, især i forhold til integration, kriminalitet og ligestilling mellem uddannelse og beskæftigelse.</t>
+          <t>To personer med kriminel baggrund er blevet forpligtet til at optages på statsborgerskabslovforslaget på grund af sagsbehandlingsfejl, hvilket rejser spørgsmål om lovens anvendelse.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Debatten om tildeling af dansk statsborgerskab fokuserer på behovet for klare retningslinjer, vurdering af ansøgeres baggrund, og overholdelse af internationale konventioner.</t>
+          <t>Der er en udbredt bekymring over indvandring og tildeling af dansk statsborgerskab, især til personer med kriminel baggrund, hvilket fører til uenighed mellem politiske partier om stramning af reglerne. Mange parter ønsker at sikre, at statsborgerskab kun gives til dem, der bidrager positivt til samfundet, og der efterlyses bedre kontrol med ansøgeres baggrund og rettigheder. Diskussionen om indvandringens omfang og dens indvirkning på det danske samfund er central, med krav om klare kriterier for tildeling af statsborgerskab.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Teksten nævner flere personer, herunder Preben Bang Henriksen, Fru Marlene Borst Hansen og Hr. Martin Henriksen.</t>
+          <t>Forhandlingen er afsluttet, da ingen ønsker at udtale sig, og der er indkaldt til afstemning. Der er stillet ændringsforslag, men ingen har ønsket at kommentere dem.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Folketinget står over for en debat om indfødsret, hvor der stilles spørgsmål ved, om internationale konventioner skal have indflydelse på beslutninger om statsborgerskab, især i forhold til personer, der kan udgøre en sikkerhedsrisiko. Der er også bekymringer om, hvordan sager behandles og beslutninger træffes i Indfødsretsudvalget, samt om det er acceptabelt at inkludere personer med problematiske baggrunde i lovforslag. Der er enighed om, at grundloven har forrang over konventionerne, og Folketinget har ret til at fastlægge betingelserne for indfødsret.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Der er en generel enighed blandt partierne om behovet for strammere kriterier for tildeling af dansk statsborgerskab, især i forhold til personer med kriminel baggrund. Der stilles spørgsmål ved, hvordan indfødsretsprocessen skal håndteres, herunder behovet for individuel behandling og objektive kriterier, samt bekymringer om politisk indflydelse på beslutningerne. Derudover er der en åbenhed for dialog og forhandlinger mellem partierne, selvom der er uenigheder om specifikke tilgange og holdninger til statsborgerskab.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Der rejses kritik af, at partier som Alternativet og Radikale Venstre ikke deltager i behandlingen af et vigtigt forslag, hvilket stiller spørgsmål ved deres seriøsitet. Liberal Alliance repræsenterer en ændring i tilgang ved at fokusere på ansøgeres værdier, hvilket skaber debat om partiets tidligere holdninger. Forhandlingen om lovforslaget er afsluttet, og det er vedtaget at henvise det til Indfødsretsudvalget.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the missing "Topic 2"
</commit_message>
<xml_diff>
--- a/output/results_llm_lda_topics.xlsx
+++ b/output/results_llm_lda_topics.xlsx
@@ -1,37 +1,111 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admkbo\Documents\FTIND\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA99824E-27B1-4A68-88ED-44C08E0CCD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>AutomatiskEmne</t>
+  </si>
+  <si>
+    <t>Der er enighed om behovet for klare og konsekvente regler for tildeling af dansk statsborgerskab og bekymringer over ændringer af betingelserne efter ansøgninger, hvilket underminerer tilliden til systemet. Diskussionen om statsborgerskab omfatter også spørgsmål om diskrimination baseret på oprindelse, økonomiske kriterier og beskyttelse af grundlæggende frihedsrettigheder. Flere partier ønsker at sikre, at borgere, der opfylder kravene, behandles retfærdigt og ikke bliver påvirket af politiske skift eller fordomme.</t>
+  </si>
+  <si>
+    <t>At opnå dansk statsborgerskab kræver opfyldelse af strenge krav, herunder sprogkundskaber, selvforsørgelse og kendskab til danske værdier, hvilket anerkendes som et stort privilegium. Fejringen af de nye statsborgere understreger vigtigheden af deres bidrag til samfundet og muligheden for at deltage aktivt i demokratiet. Der er en generel enighed om, at statsborgerskab fremmer integration og tilhørsforhold, samtidig med at der er ønsker om at lette betingelserne for at gøre det lettere for flere at blive en del af det danske fællesskab.</t>
+  </si>
+  <si>
+    <t>Der anerkendes udfordringer forbundet med islamisme og sharialov i visse ghettoer, samt problemer relateret til ikkevestlig indvandring.</t>
+  </si>
+  <si>
+    <t>Der er behov for, at politikere træffer beslutninger baseret på deres overbevisninger for at sikre Danmarks fremtid og velfærd. Regeringen anerkender forskellige synspunkter og har oprettet en ekspertgruppe for at forbedre borgerbehandlingen, men der er bekymringer om, at sindelagssamtaler kan overtræde retsstatsprincipperne. Der appelleres til ministeren om at sikre, at disse principper respekteres i statsborgerskabsansøgninger.</t>
+  </si>
+  <si>
+    <t>Indlægget kritiserer Hr. Jesper Langballes udtalelser som perfide og faktuelt mangelfulde, samtidig med at der påpeges, at direkte tiltale ikke må anvendes i debatten.</t>
+  </si>
+  <si>
+    <t>Der er behov for at nedsætte en ekspertgruppe for at opnå resultater, men der er usikkerhed om tidshorisonten. Der søges klarhed over Venstres støtte til den tidligere beslutning om en undersøgelseskommission.</t>
+  </si>
+  <si>
+    <t>Der afholdes en række taler og bemærkninger fra forskellige ordførere i Folketinget, hvor der udveksles synspunkter om udlændingepolitik, kontrol af ansøgere til statsborgerskab og politiske holdninger. Flere parter udtrykker bekymringer over håndteringen af emner såsom kriminalitet og integration, samt behovet for klarhed og ansvarlighed i lovgivningen. Der er også et fokus på samarbejde mellem partierne i den politiske debat.</t>
+  </si>
+  <si>
+    <t>Der er en stigende politisk debat om indfødsret i Danmark, med fokus på at sikre, at statsborgerskab kun tildeles personer, der har vist loyalitet og tilknytning til landet. Der er bekymring over tildelingen af statsborgerskab til personer med kriminel baggrund og et ønske om strammere kriterier og individuel vurdering af ansøgere. Partier som Dansk Folkeparti presser på for at ændre procedurerne, hvilket skaber en kompleks diskussion om balance mellem integration, sikkerhed og danske værdier.</t>
+  </si>
+  <si>
+    <t>Der har været en række afstemninger om forskellige ændringsforslag, hvor mange blev forkastet med stor margin. Lovforslaget er blevet vedtaget til direkte behandling uden fornyet udvalgsbehandling, og der er flere ændringsforslag, der er blevet betragtet som vedtaget uden afstemning, når ingen har gjort indsigelse. Generelt set har ændringsforslag fra mindretal, især fra DF, ofte ikke fået støtte fra flertallet.</t>
+  </si>
+  <si>
+    <t>Der er en fælles opfattelse af, at Socialdemokratiet lider under utilstrækkelig intern kommunikation.</t>
+  </si>
+  <si>
+    <t>Der er enighed blandt partierne om at stramme reglerne for dansk statsborgerskab, herunder krav om, at ansøgere skal dele grundlæggende demokratiske værdier og udelukkelse af personer med kriminel baggrund. Liberal Alliance og andre partier understreger behovet for at håndhæve disse stramninger og prioritere kvalificerede ansøgere.</t>
+  </si>
+  <si>
+    <t>Der er en igangværende debat om statsborgerskabslovgivning, hvor forskellige partier stiller spørgsmålstegn ved hinandens holdninger og forslag, herunder håndtering af statsløse personer og krav til ansøgere om statsborgerskab. Der er bekymring for, at massetildeling af statsborgerskaber uden tilstrækkelig kontrol kan have negative konsekvenser for samfundet, samtidig med at der er behov for at balancere demokratiske værdier med sikkerhed og integration. Diskussionen omfatter også hvordan kriminalitet påvirker tildeling af statsborgerskab og hvordan forskellige partier forholder sig til dette emne.</t>
+  </si>
+  <si>
+    <t>To personer med kriminel baggrund er blevet forpligtet til at optages på statsborgerskabslovforslaget på grund af sagsbehandlingsfejl, hvilket rejser spørgsmål om lovens anvendelse.</t>
+  </si>
+  <si>
+    <t>Der er en udbredt bekymring over indvandring og tildeling af dansk statsborgerskab, især til personer med kriminel baggrund, hvilket fører til uenighed mellem politiske partier om stramning af reglerne. Mange parter ønsker at sikre, at statsborgerskab kun gives til dem, der bidrager positivt til samfundet, og der efterlyses bedre kontrol med ansøgeres baggrund og rettigheder. Diskussionen om indvandringens omfang og dens indvirkning på det danske samfund er central, med krav om klare kriterier for tildeling af statsborgerskab.</t>
+  </si>
+  <si>
+    <t>Forhandlingen er afsluttet, da ingen ønsker at udtale sig, og der er indkaldt til afstemning. Der er stillet ændringsforslag, men ingen har ønsket at kommentere dem.</t>
+  </si>
+  <si>
+    <t>Folketinget står over for en debat om indfødsret, hvor der stilles spørgsmål ved, om internationale konventioner skal have indflydelse på beslutninger om statsborgerskab, især i forhold til personer, der kan udgøre en sikkerhedsrisiko. Der er også bekymringer om, hvordan sager behandles og beslutninger træffes i Indfødsretsudvalget, samt om det er acceptabelt at inkludere personer med problematiske baggrunde i lovforslag. Der er enighed om, at grundloven har forrang over konventionerne, og Folketinget har ret til at fastlægge betingelserne for indfødsret.</t>
+  </si>
+  <si>
+    <t>Der er en generel enighed blandt partierne om behovet for strammere kriterier for tildeling af dansk statsborgerskab, især i forhold til personer med kriminel baggrund. Der stilles spørgsmål ved, hvordan indfødsretsprocessen skal håndteres, herunder behovet for individuel behandling og objektive kriterier, samt bekymringer om politisk indflydelse på beslutningerne. Derudover er der en åbenhed for dialog og forhandlinger mellem partierne, selvom der er uenigheder om specifikke tilgange og holdninger til statsborgerskab.</t>
+  </si>
+  <si>
+    <t>Der rejses kritik af, at partier som Alternativet og Radikale Venstre ikke deltager i behandlingen af et vigtigt forslag, hvilket stiller spørgsmål ved deres seriøsitet. Liberal Alliance repræsenterer en ændring i tilgang ved at fokusere på ansøgeres værdier, hvilket skaber debat om partiets tidligere holdninger. Forhandlingen om lovforslaget er afsluttet, og det er vedtaget at henvise det til Indfødsretsudvalget.</t>
+  </si>
+  <si>
+    <t>Den kristne kulturarv i Vesteuropa er præget af sekularisme, der står i kontrast til islam som et samfundssystem, hvilket resulterer i en ukritisk accept af muslimsk indvandring.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +120,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,209 +444,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>AutomatiskEmne</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Der er enighed om behovet for klare og konsekvente regler for tildeling af dansk statsborgerskab og bekymringer over ændringer af betingelserne efter ansøgninger, hvilket underminerer tilliden til systemet. Diskussionen om statsborgerskab omfatter også spørgsmål om diskrimination baseret på oprindelse, økonomiske kriterier og beskyttelse af grundlæggende frihedsrettigheder. Flere partier ønsker at sikre, at borgere, der opfylder kravene, behandles retfærdigt og ikke bliver påvirket af politiske skift eller fordomme.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>At opnå dansk statsborgerskab kræver opfyldelse af strenge krav, herunder sprogkundskaber, selvforsørgelse og kendskab til danske værdier, hvilket anerkendes som et stort privilegium. Fejringen af de nye statsborgere understreger vigtigheden af deres bidrag til samfundet og muligheden for at deltage aktivt i demokratiet. Der er en generel enighed om, at statsborgerskab fremmer integration og tilhørsforhold, samtidig med at der er ønsker om at lette betingelserne for at gøre det lettere for flere at blive en del af det danske fællesskab.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Der anerkendes udfordringer forbundet med islamisme og sharialov i visse ghettoer, samt problemer relateret til ikkevestlig indvandring.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Der er behov for, at politikere træffer beslutninger baseret på deres overbevisninger for at sikre Danmarks fremtid og velfærd. Regeringen anerkender forskellige synspunkter og har oprettet en ekspertgruppe for at forbedre borgerbehandlingen, men der er bekymringer om, at sindelagssamtaler kan overtræde retsstatsprincipperne. Der appelleres til ministeren om at sikre, at disse principper respekteres i statsborgerskabsansøgninger.</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Indlægget kritiserer Hr. Jesper Langballes udtalelser som perfide og faktuelt mangelfulde, samtidig med at der påpeges, at direkte tiltale ikke må anvendes i debatten.</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Der er behov for at nedsætte en ekspertgruppe for at opnå resultater, men der er usikkerhed om tidshorisonten. Der søges klarhed over Venstres støtte til den tidligere beslutning om en undersøgelseskommission.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Der afholdes en række taler og bemærkninger fra forskellige ordførere i Folketinget, hvor der udveksles synspunkter om udlændingepolitik, kontrol af ansøgere til statsborgerskab og politiske holdninger. Flere parter udtrykker bekymringer over håndteringen af emner såsom kriminalitet og integration, samt behovet for klarhed og ansvarlighed i lovgivningen. Der er også et fokus på samarbejde mellem partierne i den politiske debat.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Der er en stigende politisk debat om indfødsret i Danmark, med fokus på at sikre, at statsborgerskab kun tildeles personer, der har vist loyalitet og tilknytning til landet. Der er bekymring over tildelingen af statsborgerskab til personer med kriminel baggrund og et ønske om strammere kriterier og individuel vurdering af ansøgere. Partier som Dansk Folkeparti presser på for at ændre procedurerne, hvilket skaber en kompleks diskussion om balance mellem integration, sikkerhed og danske værdier.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Der har været en række afstemninger om forskellige ændringsforslag, hvor mange blev forkastet med stor margin. Lovforslaget er blevet vedtaget til direkte behandling uden fornyet udvalgsbehandling, og der er flere ændringsforslag, der er blevet betragtet som vedtaget uden afstemning, når ingen har gjort indsigelse. Generelt set har ændringsforslag fra mindretal, især fra DF, ofte ikke fået støtte fra flertallet.</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Der er en fælles opfattelse af, at Socialdemokratiet lider under utilstrækkelig intern kommunikation.</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Der er enighed blandt partierne om at stramme reglerne for dansk statsborgerskab, herunder krav om, at ansøgere skal dele grundlæggende demokratiske værdier og udelukkelse af personer med kriminel baggrund. Liberal Alliance og andre partier understreger behovet for at håndhæve disse stramninger og prioritere kvalificerede ansøgere.</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Der er en igangværende debat om statsborgerskabslovgivning, hvor forskellige partier stiller spørgsmålstegn ved hinandens holdninger og forslag, herunder håndtering af statsløse personer og krav til ansøgere om statsborgerskab. Der er bekymring for, at massetildeling af statsborgerskaber uden tilstrækkelig kontrol kan have negative konsekvenser for samfundet, samtidig med at der er behov for at balancere demokratiske værdier med sikkerhed og integration. Diskussionen omfatter også hvordan kriminalitet påvirker tildeling af statsborgerskab og hvordan forskellige partier forholder sig til dette emne.</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>To personer med kriminel baggrund er blevet forpligtet til at optages på statsborgerskabslovforslaget på grund af sagsbehandlingsfejl, hvilket rejser spørgsmål om lovens anvendelse.</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Der er en udbredt bekymring over indvandring og tildeling af dansk statsborgerskab, især til personer med kriminel baggrund, hvilket fører til uenighed mellem politiske partier om stramning af reglerne. Mange parter ønsker at sikre, at statsborgerskab kun gives til dem, der bidrager positivt til samfundet, og der efterlyses bedre kontrol med ansøgeres baggrund og rettigheder. Diskussionen om indvandringens omfang og dens indvirkning på det danske samfund er central, med krav om klare kriterier for tildeling af statsborgerskab.</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Forhandlingen er afsluttet, da ingen ønsker at udtale sig, og der er indkaldt til afstemning. Der er stillet ændringsforslag, men ingen har ønsket at kommentere dem.</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Folketinget står over for en debat om indfødsret, hvor der stilles spørgsmål ved, om internationale konventioner skal have indflydelse på beslutninger om statsborgerskab, især i forhold til personer, der kan udgøre en sikkerhedsrisiko. Der er også bekymringer om, hvordan sager behandles og beslutninger træffes i Indfødsretsudvalget, samt om det er acceptabelt at inkludere personer med problematiske baggrunde i lovforslag. Der er enighed om, at grundloven har forrang over konventionerne, og Folketinget har ret til at fastlægge betingelserne for indfødsret.</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Der er en generel enighed blandt partierne om behovet for strammere kriterier for tildeling af dansk statsborgerskab, især i forhold til personer med kriminel baggrund. Der stilles spørgsmål ved, hvordan indfødsretsprocessen skal håndteres, herunder behovet for individuel behandling og objektive kriterier, samt bekymringer om politisk indflydelse på beslutningerne. Derudover er der en åbenhed for dialog og forhandlinger mellem partierne, selvom der er uenigheder om specifikke tilgange og holdninger til statsborgerskab.</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Der rejses kritik af, at partier som Alternativet og Radikale Venstre ikke deltager i behandlingen af et vigtigt forslag, hvilket stiller spørgsmål ved deres seriøsitet. Liberal Alliance repræsenterer en ændring i tilgang ved at fokusere på ansøgeres værdier, hvilket skaber debat om partiets tidligere holdninger. Forhandlingen om lovforslaget er afsluttet, og det er vedtaget at henvise det til Indfødsretsudvalget.</t>
-        </is>
+      <c r="B20" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>